<commit_message>
Bitácora: agregar Log y Resumen de Git/Vercel + hoja Ref Git y Vercel
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
     <sheet name="Resumen" sheetId="2" r:id="rId2"/>
+    <sheet name="Ref Git y Vercel" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -398,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -597,16 +598,67 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B12" t="str">
+        <v>14:00</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Repositorio Git en GitHub</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Crear repo fornitalia en GitHub (lucasbustosmartin-coder). git init, .gitignore (node_modules, .venv, .env), primer commit con dashboard, bitácora, scripts, SQL. Remote origin: https://github.com/lucasbustosmartin-coder/fornitalia.git. Push a rama main.</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B13" t="str">
+        <v>14:15</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Despliegue en Vercel</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Conectar cuenta GitHub a Vercel. Importar repo lucasbustosmartin-coder/fornitalia. Deploy con preset Other, sin build. App publicada en https://fornitalia.vercel.app/</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B14" t="str">
+        <v>14:20</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Raíz Vercel con vercel.json</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Crear vercel.json con rewrite: source / → destination /dashboard-flujo-caja.html. Así https://fornitalia.vercel.app/ abre directo el dashboard. Commit y push; Vercel redepliega automático.</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -767,9 +819,115 @@
         <v>Sidebar izquierdo colapsable/expandible; botón toggle (▶/◀); ítem Home por ahora; estado persistido en localStorage. Listo para ampliar con más ítems.</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Repositorio Git (GitHub)</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Repo: https://github.com/lucasbustosmartin-coder/fornitalia. Rama main. .gitignore excluye node_modules, .venv, .env. Para actualizar: git add . ; git commit -m "mensaje" ; git push origin main.</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>App en producción (Vercel)</v>
+      </c>
+      <c r="B21" t="str">
+        <v>URL pública: https://fornitalia.vercel.app/ (vercel.json reescribe / al dashboard). Cada push a main en GitHub dispara redeploy automático en Vercel. Proyecto: fornitalia, equipo Lucas Bustos, plan Hobby.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B21"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Concepto</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Valor</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Repositorio GitHub</v>
+      </c>
+      <c r="B2" t="str">
+        <v>https://github.com/lucasbustosmartin-coder/fornitalia</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>URL app en vivo (Vercel)</v>
+      </c>
+      <c r="B3" t="str">
+        <v>https://fornitalia.vercel.app/</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Rama principal</v>
+      </c>
+      <c r="B4" t="str">
+        <v>main</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Actualizar y subir cambios</v>
+      </c>
+      <c r="B5" t="str">
+        <v>git add .  →  git commit -m "descripción"  →  git push origin main</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Vercel redeploy</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Automático al hacer push a main</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Archivo configuración raíz</v>
+      </c>
+      <c r="B7" t="str">
+        <v>vercel.json (rewrite / a dashboard-flujo-caja.html)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Cuenta GitHub</v>
+      </c>
+      <c r="B8" t="str">
+        <v>lucasbustosmartin-coder</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Proyecto Vercel</v>
+      </c>
+      <c r="B9" t="str">
+        <v>fornitalia (equipo Lucas Bustos, plan Hobby)</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Regla flujo despliegue y hoja Versiones; exportar transacciones crudas; versión 1.1
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -6,6 +6,7 @@
     <sheet name="Log" sheetId="1" r:id="rId1"/>
     <sheet name="Resumen" sheetId="2" r:id="rId2"/>
     <sheet name="Ref Git y Vercel" sheetId="3" r:id="rId3"/>
+    <sheet name="Versiones" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -649,16 +650,67 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B15" t="str">
+        <v>15:00</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Exportar a Excel</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Botón "Exportar a Excel" con icono (mismo estilo que los del modal: gris, sencillo). Exporta la tabla de transacciones tal como está en Supabase: todas las columnas (fecha, mes, anio, tipo_movimiento, monto, status, medio_pago, descripcion, cliente, categoria, cat_desc, origen_archivo, cuenta_contable) en una hoja Excel para poder analizar los datos desde Excel. Librería SheetJS (xlsx) en el navegador.</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B16" t="str">
+        <v>15:10</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Exportar transacciones crudas</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Ajuste: el botón Exportar a Excel pasa a exportar directamente la tabla de transacciones (datos crudos de Supabase), no el resumen flujo por mes, para permitir manipular y analizar los datos desde Excel.</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B17" t="str">
+        <v>15:30</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Regla flujo despliegue y versiones</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Nueva regla: al final de cada tarea el usuario prueba en local y confirma; recién entonces el asistente despliega (git push). Se agrega hoja Versiones en la bitácora para registrar versión incremental en cada despliegue (1.0, 1.1, …).</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E17"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -835,9 +887,33 @@
         <v>URL pública: https://fornitalia.vercel.app/ (vercel.json reescribe / al dashboard). Cada push a main en GitHub dispara redeploy automático en Vercel. Proyecto: fornitalia, equipo Lucas Bustos, plan Hobby.</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Exportar a Excel</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Botón en la barra de la tabla (solo icono). Exporta la tabla de transacciones tal como está en Supabase: una hoja "Transacciones" con columnas fecha, mes, anio, tipo_movimiento, monto, status, medio_pago, descripcion, cliente, categoria, cat_desc, origen_archivo, cuenta_contable. Permite analizar y manipular los datos desde Excel.</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Flujo de despliegue</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Al terminar cada tarea: el usuario prueba en local y confirma; recién entonces el asistente hace git add, commit y push (Vercel redepliega automático). No se despliega hasta confirmación.</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Versiones en bitácora</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Hoja "Versiones" en Bitacora_tareas.xlsx: registro incremental (1.0, 1.1, …) con fecha y descripción de cada despliegue a Git/Vercel.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B24"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -930,4 +1006,56 @@
     <ignoredError numberStoredAsText="1" sqref="A1:B9"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="75.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Versión</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Fecha</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Descripción</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Estado inicial: dashboard flujo de caja, exportar transacciones a Excel, despliegue en Vercel</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Regla flujo despliegue (probar en local → confirmar → desplegar); hoja Versiones en bitácora</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mejorar modal detalle (tabla, moneda, TC) y normalizar moneda
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -701,16 +701,84 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B18" t="str">
+        <v>16:00</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Campo moneda en tabla transacciones</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Agregar columna moneda (ARS/USD) a la tabla transacciones en Supabase para normalizar la moneda de registración. Migración en supabase_transacciones_moneda.sql. Dashboard prioriza moneda; si viene vacío, infiere desde medio_pago. Export a Excel incluye columna moneda.</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B19" t="str">
+        <v>16:20</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Modal detalle: ancho y moneda registración</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Ensanchado del modal mensual de detalle. En el listado de transacciones se muestra el monto con su moneda de registración (US$ / $) antes del monto; si difiere de la moneda seleccionada, se muestra la conversión a la moneda de vista (→) o (sin cot.) si falta tipo de cambio.</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B20" t="str">
+        <v>16:30</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Modal detalle: transacciones en tabla</v>
+      </c>
+      <c r="D20" t="str">
+        <v>En el modal mensual (By Categoría / By Cuenta), el detalle expandido de transacciones ahora se renderiza como una tabla con encabezados (Fecha, Tipo, Medio, Mon., Monto, moneda vista, Descripción, Origen) para una lectura y análisis más clara.</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B21" t="str">
+        <v>16:40</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Modal detalle: columna TC</v>
+      </c>
+      <c r="D21" t="str">
+        <v>En la tabla de detalle expandida del modal mensual se agrega columna TC (MEP/CCL/OFICIAL según selector). Se muestra el tipo de cambio aplicado por fecha cuando hay conversión entre moneda de registración y moneda de vista; si no aplica muestra — y si falta cotización muestra sin cot.</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E21"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -833,87 +901,119 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Alertas por mes</v>
+        <v>Detalle transacciones (moneda registración)</v>
       </c>
       <c r="B15" t="str">
-        <v>Avisos: mes sin egresos; sin registros de Sueldos, Comisiones, Alquileres o Impuestos; desvío % de categoría vs mes anterior.</v>
+        <v>En el modal mensual, cada línea muestra el monto en su moneda de registración (US$ / $). Si la moneda seleccionada difiere, se muestra la conversión a la moneda de vista (→) o indica (sin cot.) si falta tipo de cambio.</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Sin cotización</v>
+        <v>Detalle transacciones (tabla)</v>
       </c>
       <c r="B16" t="str">
-        <v>Pestaña con transacciones que no tienen tipo de cambio (excluidas del resumen).</v>
+        <v>En el modal mensual, al expandir una categoría/cuenta se muestra una tabla con títulos y filas de transacciones (Fecha, Tipo, Medio, Moneda, Monto, moneda vista, Descripción, Origen).</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Exclusiones</v>
+        <v>Detalle transacciones (tipo de cambio)</v>
       </c>
       <c r="B17" t="str">
-        <v>No se incluyen transacciones anuladas ni categorías Apertura y Cierre.</v>
+        <v>En el detalle expandido del modal mensual, se muestra la columna TC (según MEP/CCL/Oficial) cuando hay conversión entre moneda registración y moneda vista; si no aplica muestra — y si falta cotización muestra sin cot.</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Datos</v>
+        <v>Alertas por mes</v>
       </c>
       <c r="B18" t="str">
-        <v>Transacciones y tipo de cambio desde Supabase. Cotización faltante: se usa la fecha anterior disponible.</v>
+        <v>Avisos: mes sin egresos; sin registros de Sueldos, Comisiones, Alquileres o Impuestos; desvío % de categoría vs mes anterior.</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Menú lateral</v>
+        <v>Sin cotización</v>
       </c>
       <c r="B19" t="str">
-        <v>Sidebar izquierdo colapsable/expandible; botón toggle (▶/◀); ítem Home por ahora; estado persistido en localStorage. Listo para ampliar con más ítems.</v>
+        <v>Pestaña con transacciones que no tienen tipo de cambio (excluidas del resumen).</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Repositorio Git (GitHub)</v>
+        <v>Exclusiones</v>
       </c>
       <c r="B20" t="str">
-        <v>Repo: https://github.com/lucasbustosmartin-coder/fornitalia. Rama main. .gitignore excluye node_modules, .venv, .env. Para actualizar: git add . ; git commit -m "mensaje" ; git push origin main.</v>
+        <v>No se incluyen transacciones anuladas ni categorías Apertura y Cierre.</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>App en producción (Vercel)</v>
+        <v>Datos</v>
       </c>
       <c r="B21" t="str">
-        <v>URL pública: https://fornitalia.vercel.app/ (vercel.json reescribe / al dashboard). Cada push a main en GitHub dispara redeploy automático en Vercel. Proyecto: fornitalia, equipo Lucas Bustos, plan Hobby.</v>
+        <v>Transacciones y tipo de cambio desde Supabase. Cotización faltante: se usa la fecha anterior disponible.</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Exportar a Excel</v>
+        <v>Menú lateral</v>
       </c>
       <c r="B22" t="str">
-        <v>Botón en la barra de la tabla (solo icono). Exporta la tabla de transacciones tal como está en Supabase: una hoja "Transacciones" con columnas fecha, mes, anio, tipo_movimiento, monto, status, medio_pago, descripcion, cliente, categoria, cat_desc, origen_archivo, cuenta_contable. Permite analizar y manipular los datos desde Excel.</v>
+        <v>Sidebar izquierdo colapsable/expandible; botón toggle (▶/◀); ítem Home por ahora; estado persistido en localStorage. Listo para ampliar con más ítems.</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Flujo de despliegue</v>
+        <v>Repositorio Git (GitHub)</v>
       </c>
       <c r="B23" t="str">
-        <v>Al terminar cada tarea: el usuario prueba en local y confirma; recién entonces el asistente hace git add, commit y push (Vercel redepliega automático). No se despliega hasta confirmación.</v>
+        <v>Repo: https://github.com/lucasbustosmartin-coder/fornitalia. Rama main. .gitignore excluye node_modules, .venv, .env. Para actualizar: git add . ; git commit -m "mensaje" ; git push origin main.</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
+        <v>App en producción (Vercel)</v>
+      </c>
+      <c r="B24" t="str">
+        <v>URL pública: https://fornitalia.vercel.app/ (vercel.json reescribe / al dashboard). Cada push a main en GitHub dispara redeploy automático en Vercel. Proyecto: fornitalia, equipo Lucas Bustos, plan Hobby.</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Exportar a Excel</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Botón en la barra de la tabla (solo icono). Exporta la tabla de transacciones tal como está en Supabase: una hoja "Transacciones" con columnas fecha, mes, anio, tipo_movimiento, monto, status, medio_pago, descripcion, cliente, categoria, cat_desc, origen_archivo, cuenta_contable. Permite analizar y manipular los datos desde Excel.</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Flujo de despliegue</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Al terminar cada tarea: el usuario prueba en local y confirma; recién entonces el asistente hace git add, commit y push (Vercel redepliega automático). No se despliega hasta confirmación.</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
         <v>Versiones en bitácora</v>
       </c>
-      <c r="B24" t="str">
+      <c r="B27" t="str">
         <v>Hoja "Versiones" en Bitacora_tareas.xlsx: registro incremental (1.0, 1.1, …) con fecha y descripción de cada despliegue a Git/Vercel.</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Campo moneda (BD)</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Columna moneda en tabla transacciones (ARS/USD). Si está informada, el dashboard la usa; si no, infiere desde medio_pago (ej. "dolar" → USD). Export a Excel incluye moneda.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B24"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B28"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1010,7 +1110,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1053,9 +1153,20 @@
         <v>Regla flujo despliegue (probar en local → confirmar → desplegar); hoja Versiones en bitácora</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Modal mensual: detalle en tabla + moneda registración + TC; normalización moneda en BD y export Excel con moneda</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Errores de clasificación: solapa, edición y flags
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -769,16 +769,67 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B22" t="str">
+        <v>16:50</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Recategorización Alquiler → Alquileres y Servicios</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Si la categoría original es exactamente Alquiler, el dashboard la muestra como Alquileres y Servicios (solo cambio de etiqueta visual, los números y agrupaciones siguen conciliando).</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B23" t="str">
+        <v>17:00</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Detección de errores de clasificación (Egresos)</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Para egresos: si la descripción (más cat_desc/cliente) no contiene palabras relevantes de la categoría mostrada o de la cuenta contable, se recategoriza visualmente como Sin categoría y se registra como error de tipo "Inconsistencia entre Categoria , Cuenta Contable y Descripcion". En el modal mensual se agrega solapa Errores con el conteo y un acceso a un modal de detalle con todos los registros en error.</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B24" t="str">
+        <v>17:30</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Modal errores: ampliar, editar registro y campos editado/editado_detalle</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Ampliar modal de detalle de errores. Agregar icono de edición por registro que abre modal para actualizar en BD: Categoría y Cuenta contable solo desde valores existentes (dropdown), Descripción libre. Tabla transacciones: nuevos campos editado (flag) y editado_detalle (ej. Categoria, Descripcion, Cuenta Contable). Migración supabase_transacciones_editado.sql. Export Excel incluye editado y editado_detalle.</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E24"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1011,9 +1062,25 @@
         <v>Columna moneda en tabla transacciones (ARS/USD). Si está informada, el dashboard la usa; si no, infiere desde medio_pago (ej. "dolar" → USD). Export a Excel incluye moneda.</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Edición desde modal Errores</v>
+      </c>
+      <c r="B29" t="str">
+        <v>En el detalle de errores, icono de edición por registro. Abre modal para corregir: Categoría y Cuenta contable solo desde valores existentes en BD; Descripción libre. Al guardar se actualiza la fila y se marcan editado y editado_detalle (qué campos se editaron).</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Campos editado y editado_detalle</v>
+      </c>
+      <c r="B30" t="str">
+        <v>En transacciones: editado (boolean) y editado_detalle (texto, ej. "Categoria, Descripcion, Cuenta Contable"). Migración supabase_transacciones_editado.sql. Export Excel los incluye.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B28"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B30"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Excepciones errores: Comisiones Bancarias, Impuestos/MercadoPago y Morba, Alquiler; versión 1.3
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -820,9 +820,60 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B25" t="str">
+        <v>17:40</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Excepción errores: Comisiones Bancarias / Gastos Bancarios</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Si la categoría es Comisiones Bancarias y la cuenta contable es Gastos Bancarios, se considera consistente y no entra en el log de errores de clasificación (aunque la descripción no contenga esas palabras).</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B26" t="str">
+        <v>17:50</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Excepción errores: Impuestos / MercadoPago y Impuestos / Transferencia Morba</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Si la categoría es Impuestos y la cuenta contable es MercadoPago o Transferencia Morba, se considera consistente y no entra en el log de errores de clasificación, aunque la descripción no contenga esas palabras.</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B27" t="str">
+        <v>18:00</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Excepción errores: Alquileres y Servicios / Alquiler</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Si la categoría es Alquiler (mostrada como Alquileres y Servicios) y la cuenta contable es Alquiler, se considera consistente y no entra en el log de errores de clasificación.</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E24"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E27"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1177,7 +1228,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1231,9 +1282,20 @@
         <v>Modal mensual: detalle en tabla + moneda registración + TC; normalización moneda en BD y export Excel con moneda</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B5" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Errores de clasificación (solapa Errores), edición desde modal, editado/editado_detalle; excepciones: Comisiones Bancarias/Gastos Bancarios, Impuestos/MercadoPago y Transferencia Morba, Alquiler/Alquiler</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.4: monto numérico en exportación Excel; regla bitácora por defecto
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -7,6 +7,7 @@
     <sheet name="Resumen" sheetId="2" r:id="rId2"/>
     <sheet name="Ref Git y Vercel" sheetId="3" r:id="rId3"/>
     <sheet name="Versiones" sheetId="4" r:id="rId4"/>
+    <sheet name="Presupuesto" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -400,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -871,9 +872,43 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B28" t="str">
+        <v>18:10</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Solapa Errores global y exportación a Excel</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Nueva pestaña Errores en el dashboard (a la derecha de Sin cotización) que lista todos los egresos con error de clasificación, permite editar cada registro con el mismo modal de edición y se puede exportar a Excel con todos los campos relevantes (incluyendo editado y editado_detalle).</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B29" t="str">
+        <v>18:20</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Monto numérico en exportación Excel</v>
+      </c>
+      <c r="D29" t="str">
+        <v>En ambas exportaciones (Transacciones y Errores), la columna monto se escribe como valor numérico (Number) en lugar de texto, para que Excel reconozca números y permita usar fórmulas (SUM, SUMIF, etc.).</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E29"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1086,7 +1121,7 @@
         <v>Exportar a Excel</v>
       </c>
       <c r="B25" t="str">
-        <v>Botón en la barra de la tabla (solo icono). Exporta la tabla de transacciones tal como está en Supabase: una hoja "Transacciones" con columnas fecha, mes, anio, tipo_movimiento, monto, status, medio_pago, descripcion, cliente, categoria, cat_desc, origen_archivo, cuenta_contable. Permite analizar y manipular los datos desde Excel.</v>
+        <v>Botón en la barra de la tabla (solo icono). Exporta la tabla de transacciones tal como está en Supabase: una hoja "Transacciones" con columnas fecha, mes, anio, tipo_movimiento, monto (valor numérico para fórmulas), status, medio_pago, moneda, descripcion, cliente, categoria, cat_desc, origen_archivo, cuenta_contable, editado, editado_detalle. Export Errores: monto también como número. Permite analizar y usar fórmulas en Excel.</v>
       </c>
     </row>
     <row r="26">
@@ -1228,7 +1263,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1293,9 +1328,105 @@
         <v>Errores de clasificación (solapa Errores), edición desde modal, editado/editado_detalle; excepciones: Comisiones Bancarias/Gastos Bancarios, Impuestos/MercadoPago y Transferencia Morba, Alquiler/Alquiler</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="B6" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Exportación Excel: monto como valor numérico (fórmulas en Excel); regla bitácora por defecto reforzada</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="90.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Grupo</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Descripción comercial</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Importe sugerido (ARS)</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Normalización de datos</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Relevamiento, limpieza y normalización de datos históricos de caja (campos de moneda, categorías, cuentas contables, flags de edición). Incluye lógica de excepciones y detección de inconsistencias.</v>
+      </c>
+      <c r="C2">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Dashboard flujo de caja</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Diseño y desarrollo del dashboard mensual (Flujo por mes, Resumen, alertas, modal By Categoría / By Cuenta, gráficos de serie mensual). Incluye formatos de moneda y visualizaciones.</v>
+      </c>
+      <c r="C3">
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Bitácora y documentación</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Implementación de la bitácora en Excel (Log, Resumen, Versiones, Ref Git y Vercel, Presupuesto) y documentación funcional básica para el uso de la app.</v>
+      </c>
+      <c r="C4">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Integración y despliegue</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Configuración de repositorio Git/GitHub, flujo de despliegue a Vercel y ajustes de configuración (vercel.json, conexión con Supabase).</v>
+      </c>
+      <c r="C5">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Mantenimiento y soporte inicial</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Soporte post–implementación, pequeños ajustes funcionales y acompañamiento durante el primer período de uso.</v>
+      </c>
+      <c r="C6">
+        <v>80000</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.5: tipo de error, duplicados (cliente igual), filtro errores, modal con id_origen, timeout carga
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -906,16 +906,67 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B30" t="str">
+        <v>18:30</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Tipo de error y detección de potencial duplicado</v>
+      </c>
+      <c r="D30" t="str">
+        <v>En la solapa Errores: columna Tipo de error (Inconsistencia entre Categoria/Cuenta/Descripcion o Potencial registro duplicado). Detección de duplicados por misma fecha, monto, tipo_movimiento y descripción similar. Para duplicados: icono Ver que abre modal comparando ambos registros; opciones Excluir de cálculos (anular) o Eliminar registro. Export Excel incluye tipo_error.</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B31" t="str">
+        <v>18:40</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Filtro por tipo de error en solapa Errores</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Selector "Tipo de error" en la barra de la solapa Errores: Todos, Inconsistencia (categoría/cuenta/descripción), Potencial registro duplicado. La tabla y la exportación a Excel respetan el filtro seleccionado.</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B32" t="str">
+        <v>18:50</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Duplicados: cliente igual e id_origen en comparación</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Solo se marca potencial duplicado si además de fecha, monto, tipo y descripción similar el campo cliente es igual; si cliente es distinto no se marca. En el modal de comparación (Este registro / Posible duplicado) se incluye id_origen y Cliente.</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E32"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1164,9 +1215,41 @@
         <v>En transacciones: editado (boolean) y editado_detalle (texto, ej. "Categoria, Descripcion, Cuenta Contable"). Migración supabase_transacciones_editado.sql. Export Excel los incluye.</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Tipo de error en Errores</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Tabla de errores muestra columna Tipo de error: Inconsistencia entre Categoria, Cuenta Contable y Descripcion; o Potencial registro duplicado. Export a Excel incluye tipo_error.</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Detección de potencial duplicado</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Registros con misma fecha, monto, tipo_movimiento y descripción similar se marcan como potencial duplicado. Icono Ver abre modal con comparación Este registro / Posible duplicado; acciones: Excluir de cálculos (anular) o Eliminar registro.</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Filtro por tipo de error</v>
+      </c>
+      <c r="B33" t="str">
+        <v>En la solapa Errores, selector para filtrar por tipo: Todos, Inconsistencia (categoría/cuenta/descripción), Potencial registro duplicado. La exportación a Excel exporta solo los registros visibles según el filtro.</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Duplicados: condición cliente</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Dos registros son potencial duplicado solo si coinciden en fecha, monto, tipo_movimiento, descripción similar y además cliente es igual; si cliente es distinto no se marcan como duplicado. Modal de comparación muestra id_origen y Cliente.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B34"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1263,7 +1346,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1339,9 +1422,20 @@
         <v>Exportación Excel: monto como valor numérico (fórmulas en Excel); regla bitácora por defecto reforzada</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="B7" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Errores: tipo de error, detección duplicados (cliente igual), filtro por tipo, modal comparación con id_origen; timeout carga y fechaStr para fechas</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.6: botones Excel verde, Evolución ingreso/egreso, modal detalle con Origen y más ancho
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -957,16 +957,101 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B33" t="str">
+        <v>19:00</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Regla bitácora: actualizar todas las solapas necesarias</v>
+      </c>
+      <c r="D33" t="str">
+        <v>La regla pasa a exigir actualizar todas las solapas que correspondan: Log, Resumen (si aplica), Presupuesto (cuando la tarea agrega o cambia un entregable comercial), Versiones (en despliegue). Presupuesto se actualiza con el rubro "Detección de duplicados y gestión de errores".</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B34" t="str">
+        <v>19:10</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Solapa Evolución (tabla dinámica)</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Nueva pestaña Evolución: tabla dinámica con Agrupar por (Categoría o Cuenta contable) como fila y Período (Diario o Mensual) como columna. Diario muestra fecha (día), Mensual muestra MM-YYYY. Celdas = neto (ingresos - egresos) en la moneda seleccionada. Columna Total por fila.</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B35" t="str">
+        <v>19:20</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Evolución: clic en valor y exportar a Excel</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Al hacer clic en un valor de la tabla Evolución se abre un modal con detalle mínimo: Fecha, Categoría, Descripción, Monto (registros que componen esa celda). Botón Exportar Evolución a Excel exporta la tabla resultante según los filtros Agrupar por y Período.</v>
+      </c>
+      <c r="E35" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B36" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Exportaciones: título moneda, icono Excel, Exportar Base Histórica</v>
+      </c>
+      <c r="D36" t="str">
+        <v>En todas las exportaciones a Excel se agrega una fila título que indica la moneda (o que ver columna moneda). Icono tipo Excel (tabla/grid) en botones de exportar. Exportar base de transacciones movido a la línea del selector de moneda con título "Exportar Base Histórica" e icono Excel; mismo icono en Exportar Evolución a Excel.</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B37" t="str">
+        <v>19:40</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Evolución: ingreso primero, luego egreso</v>
+      </c>
+      <c r="D37" t="str">
+        <v>En la tabla Evolución las filas (categorías o cuentas) se ordenan primero las de ingreso (total &gt;= 0) y luego las de egreso (total &lt; 0); dentro de cada grupo orden alfabético.</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E32"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E37"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1247,9 +1332,49 @@
         <v>Dos registros son potencial duplicado solo si coinciden en fecha, monto, tipo_movimiento, descripción similar y además cliente es igual; si cliente es distinto no se marcan como duplicado. Modal de comparación muestra id_origen y Cliente.</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Regla bitácora</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Actualizar todas las solapas necesarias: Log (siempre que haya tarea), Resumen (si cambia funcionalidad), Presupuesto (si agrega o cambia entregable comercial), Versiones (en despliegue). Regenerar Excel tras editar crear-bitacora-excel.js.</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Evolución (tabla dinámica)</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Solapa Evolución: Agrupar por = Categoría o Cuenta contable (fila); Período = Diario (fecha por día) o Mensual (MM-YYYY). Columnas = períodos, celdas = neto en moneda seleccionada, columna Total.</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Evolución: detalle al clic y exportar</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Clic en un valor de la tabla Evolución abre modal con detalle: Fecha, Categoría, Descripción, Monto. Exportar Evolución a Excel exporta la tabla según filtros Agrupar por y Período.</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Exportaciones Excel</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Todas las exportaciones incluyen una fila título con la moneda. Exportar Base Histórica (icono Excel) en la línea del selector de moneda; Exportar Evolución a Excel con el mismo icono.</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Evolución: orden ingreso/egreso</v>
+      </c>
+      <c r="B39" t="str">
+        <v>En la tabla Evolución las filas se muestran primero las de ingreso (total &gt;= 0) y luego las de egreso (total &lt; 0); dentro de cada grupo orden alfabético. Aplica tanto al agrupar por Categoría como por Cuenta contable.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B34"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B39"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1346,7 +1471,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1433,16 +1558,27 @@
         <v>Errores: tipo de error, detección duplicados (cliente igual), filtro por tipo, modal comparación con id_origen; timeout carga y fechaStr para fechas</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>1.6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Export Excel: botones verde y blanco; Evolución: orden ingreso luego egreso; modal detalle Evolución con columna Origen y modal más ancho</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1487,40 +1623,62 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Bitácora y documentación</v>
+        <v>Detección de duplicados y gestión de errores</v>
       </c>
       <c r="B4" t="str">
-        <v>Implementación de la bitácora en Excel (Log, Resumen, Versiones, Ref Git y Vercel, Presupuesto) y documentación funcional básica para el uso de la app.</v>
+        <v>Detección de potencial duplicado (fecha, monto, tipo, cliente, descripción similar), tipo de error (inconsistencia / duplicado), filtro por tipo, modal de comparación con id_origen y Cliente, acciones anular o eliminar registro.</v>
       </c>
       <c r="C4">
-        <v>120000</v>
+        <v>85000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Integración y despliegue</v>
+        <v>Evolución (tabla dinámica)</v>
       </c>
       <c r="B5" t="str">
-        <v>Configuración de repositorio Git/GitHub, flujo de despliegue a Vercel y ajustes de configuración (vercel.json, conexión con Supabase).</v>
+        <v>Solapa Evolución: tabla dinámica con filas por Categoría o Cuenta contable y columnas por Período (Diario o Mensual). Neto por celda en moneda seleccionada.</v>
       </c>
       <c r="C5">
-        <v>90000</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>Bitácora y documentación</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Implementación de la bitácora en Excel (Log, Resumen, Versiones, Ref Git y Vercel, Presupuesto) y documentación funcional básica para el uso de la app.</v>
+      </c>
+      <c r="C6">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Integración y despliegue</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Configuración de repositorio Git/GitHub, flujo de despliegue a Vercel y ajustes de configuración (vercel.json, conexión con Supabase).</v>
+      </c>
+      <c r="C7">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
         <v>Mantenimiento y soporte inicial</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B8" t="str">
         <v>Soporte post–implementación, pequeños ajustes funcionales y acompañamiento durante el primer período de uso.</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>80000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.7: Solapa Errores - columna Mes-Año reemplazada por Id_Origen
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1042,9 +1042,26 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B38" t="str">
+        <v>19:50</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Solapa Errores: columna Mes-Año por Id_Origen</v>
+      </c>
+      <c r="D38" t="str">
+        <v>En la tabla de la solapa Errores se reemplaza la columna Mes-Año por Id_Origen (identificador de origen del registro).</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E37"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E38"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1471,7 +1488,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1569,9 +1586,20 @@
         <v>Export Excel: botones verde y blanco; Evolución: orden ingreso luego egreso; modal detalle Evolución con columna Origen y modal más ancho</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>1.7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Solapa Errores: columna Mes-Año reemplazada por Id_Origen en la tabla</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.8: Balance → G/P; modal Evolución con Id_Origen
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1059,9 +1059,26 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B39" t="str">
+        <v>20:00</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Balance por G/P e Id_Origen en modal Evolución</v>
+      </c>
+      <c r="D39" t="str">
+        <v>En todo el dashboard se reemplaza la etiqueta Balance por G/P (Ganancia/Pérdida). En el modal de detalle al hacer clic en un valor de Evolución se agrega la columna Id_Origen.</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E39"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1488,7 +1505,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1597,9 +1614,20 @@
         <v>Solapa Errores: columna Mes-Año reemplazada por Id_Origen en la tabla</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>1.8</v>
+      </c>
+      <c r="B10" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Balance reemplazado por G/P (Ganancia/Pérdida); modal detalle Evolución con columna Id_Origen</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.9: Comisiones solo cat. Comisiones; Total flujo por mes; Errores sin Editado, scroll, Descripción izq.
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1076,9 +1076,26 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B40" t="str">
+        <v>20:10</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Comisiones, Total flujo, Errores</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Comisiones solo categoría Comisiones (no Sueldos). Fila Total en flujo por mes con sumas y ratios. Tabla Errores: quitar columna Editado, scroll horizontal, Descripción alineada a la izquierda.</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E40"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1505,7 +1522,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1625,9 +1642,20 @@
         <v>Balance reemplazado por G/P (Ganancia/Pérdida); modal detalle Evolución con columna Id_Origen</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>1.9</v>
+      </c>
+      <c r="B11" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Comisiones solo categoría Comisiones; fila Total en flujo por mes; Errores: sin columna Editado, scroll horizontal, Descripción a la izquierda</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.10: Base histórica id_origen/id_operacion; versión en sidebar; regla versionado al desplegar
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1093,9 +1093,26 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B41" t="str">
+        <v>20:20</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Base histórica Excel y versión en sidebar</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Export Base histórica: columnas id_origen e id_operacion. Versión de la app visible abajo en el sidebar (APP_VERSION). Regla de bitácora: al indicar desplegar, incrementar versión, actualizar bitácora y desplegar.</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E40"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E41"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1522,7 +1539,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1653,9 +1670,20 @@
         <v>Comisiones solo categoría Comisiones; fila Total en flujo por mes; Errores: sin columna Editado, scroll horizontal, Descripción a la izquierda</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>1.10</v>
+      </c>
+      <c r="B12" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Base histórica Excel: id_origen e id_operacion; versión en sidebar; regla de versionado al desplegar</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.11: Comisiones/Ventas % con Comisiones + Sueldos (Comisiones Ventas); misma regla en modal
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1110,9 +1110,26 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="B42" t="str">
+        <v>09:15</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Comisiones/Ventas % y modal By Categoría</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Ratio Comisiones/Ventas % incluye categoría Comisiones y Sueldos con descripción Comisiones Ventas (comision/comisones). Modal By Categoría ya usaba getCategoriaDisplay con la misma regla.</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E42"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1539,7 +1556,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1681,9 +1698,20 @@
         <v>Base histórica Excel: id_origen e id_operacion; versión en sidebar; regla de versionado al desplegar</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>1.11</v>
+      </c>
+      <c r="B13" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Comisiones/Ventas %: categoría Comisiones + Sueldos (Comisiones Ventas); misma regla en modal By Categoría</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C13"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.12: Favicon L&P (azul oscuro, texto blanco) en pestaña del navegador
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1127,9 +1127,26 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="B43" t="str">
+        <v>09:30</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Favicon L&amp;P en pestaña del navegador</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Favicon favicon.svg: círculo azul oscuro (#0d2137), texto L&amp;P en blanco, más grande. Enlace en dashboard para que se vea en la solapa del explorador.</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Diagnostico</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E43"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1556,7 +1573,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1709,9 +1726,20 @@
         <v>Comisiones/Ventas %: categoría Comisiones + Sueldos (Comisiones Ventas); misma regla en modal By Categoría</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>1.12</v>
+      </c>
+      <c r="B14" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Favicon L&amp;P: ícono en pestaña del navegador (fondo azul oscuro, texto blanco)</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.13: Int. por caución, carga Excel al refrescar, modal marcha de cálculo, G/P acum + interés acum
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1144,16 +1144,33 @@
         <v>Diagnostico</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="B44" t="str">
+        <v>21:00</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Int. por caución y marcha de cálculo</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Columna Int. por caución en flujo por mes: interés por reinvertir sobrante a un día con tasa de Serie_Cauciones. Carga Excel Serie_Cauciones.xlsx al refrescar (o fallback serie_cauciones.json). Modal al clic en valor mensual con marcha: G/P acum, Int T-1, Base, Tasa, Int T. Cálculo sobre G/P acumulado a la fecha + interés acumulado (reinversión día a día). Fechas ISO (2025-08-25T00:00:00) y columna tasa_diaria.</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Implementacion</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E43"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E44"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1474,9 +1491,17 @@
         <v>En la tabla Evolución las filas se muestran primero las de ingreso (total &gt;= 0) y luego las de egreso (total &lt; 0); dentro de cada grupo orden alfabético. Aplica tanto al agrupar por Categoría como por Cuenta contable.</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Int. por caución</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Columna en flujo por mes: interés mensual por colocar el sobrante de caja a la tasa diaria de la serie de cauciones. Carga Serie_Cauciones.xlsx al refrescar (o serie_cauciones.json si no hay Excel). Cálculo: base = G/P acumulado a la fecha + interés acumulado; Int T = base × tasa. Clic en el valor abre modal con marcha (G/P acum, Int T-1, Base, Tasa, Int T).</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B40"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1573,7 +1598,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1737,9 +1762,20 @@
         <v>Favicon L&amp;P: ícono en pestaña del navegador (fondo azul oscuro, texto blanco)</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>1.13</v>
+      </c>
+      <c r="B15" t="str">
+        <v>27/02/2025</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Int. por caución: columna en flujo, carga Excel al refrescar, modal marcha de cálculo (G/P acum, Base, Tasa, Int T), cálculo sobre G/P acum + interés acum</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Bitácora: Presupuesto - rubro Int. por caución
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -1782,7 +1782,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1849,40 +1849,51 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Bitácora y documentación</v>
+        <v>Interés por caución</v>
       </c>
       <c r="B6" t="str">
-        <v>Implementación de la bitácora en Excel (Log, Resumen, Versiones, Ref Git y Vercel, Presupuesto) y documentación funcional básica para el uso de la app.</v>
+        <v>Columna Int. por caución en flujo por mes: cálculo de interés mensual por reinversión del sobrante a un día con tasa de serie de cauciones. Carga de Excel al refrescar, modal de marcha de cálculo (G/P acum, Base, Tasa, Int T). Incluye soporte para múltiples formatos de fecha y columna tasa_diaria.</v>
       </c>
       <c r="C6">
-        <v>120000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Integración y despliegue</v>
+        <v>Bitácora y documentación</v>
       </c>
       <c r="B7" t="str">
-        <v>Configuración de repositorio Git/GitHub, flujo de despliegue a Vercel y ajustes de configuración (vercel.json, conexión con Supabase).</v>
+        <v>Implementación de la bitácora en Excel (Log, Resumen, Versiones, Ref Git y Vercel, Presupuesto) y documentación funcional básica para el uso de la app.</v>
       </c>
       <c r="C7">
-        <v>90000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>Integración y despliegue</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Configuración de repositorio Git/GitHub, flujo de despliegue a Vercel y ajustes de configuración (vercel.json, conexión con Supabase).</v>
+      </c>
+      <c r="C8">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
         <v>Mantenimiento y soporte inicial</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B9" t="str">
         <v>Soporte post–implementación, pequeños ajustes funcionales y acompañamiento durante el primer período de uso.</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>80000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.14: Solapa Todas las transacciones, modal edición completa con combos
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1161,16 +1161,33 @@
         <v>Implementacion</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="B45" t="str">
+        <v>12:00</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Solapa Todas las transacciones y edición completa</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Nueva solapa Todas las transacciones: listado con todas las columnas, filtros por mes y categoría, botón Editar por registro. Modal de edición ampliado: todos los campos editables; combos para valores normalizados (categoría, cuenta contable, tipo movimiento, status, medio pago, moneda, origen archivo). editado y editado_detalle al guardar.</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Implementacion</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E44"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E45"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1499,9 +1516,25 @@
         <v>Columna en flujo por mes: interés mensual por colocar el sobrante de caja a la tasa diaria de la serie de cauciones. Carga Serie_Cauciones.xlsx al refrescar (o serie_cauciones.json si no hay Excel). Cálculo: base = G/P acumulado a la fecha + interés acumulado; Int T = base × tasa. Clic en el valor abre modal con marcha (G/P acum, Int T-1, Base, Tasa, Int T).</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Todas las transacciones</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Solapa que lista todas las transacciones con todas las columnas. Filtros por mes y categoría. Botón Editar por registro abre modal de edición completa.</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Edición completa de registros</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Modal de edición con todos los campos: fecha, mes, año, tipo movimiento, monto, moneda, status, medio pago, categoría, cuenta contable, origen archivo, descripción, cliente, cat_desc, id_origen, id_operación. Combos para campos normalizados (valores existentes en BD). editado y editado_detalle al guardar.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B40"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B42"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1598,7 +1631,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1773,16 +1806,27 @@
         <v>Int. por caución: columna en flujo, carga Excel al refrescar, modal marcha de cálculo (G/P acum, Base, Tasa, Int T), cálculo sobre G/P acum + interés acum</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>1.14</v>
+      </c>
+      <c r="B16" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Solapa Todas las transacciones (filtros mes y categoría); modal edición completa con todos los campos y combos para normalizados</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C16"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1860,40 +1904,51 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Bitácora y documentación</v>
+        <v>Listado y edición completa de transacciones</v>
       </c>
       <c r="B7" t="str">
-        <v>Implementación de la bitácora en Excel (Log, Resumen, Versiones, Ref Git y Vercel, Presupuesto) y documentación funcional básica para el uso de la app.</v>
+        <v>Solapa Todas las transacciones con listado completo, filtros por mes y categoría, y modal de edición con todos los campos y combos para valores normalizados (categoría, cuenta contable, tipo movimiento, status, medio pago, moneda, origen archivo).</v>
       </c>
       <c r="C7">
-        <v>120000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Integración y despliegue</v>
+        <v>Bitácora y documentación</v>
       </c>
       <c r="B8" t="str">
-        <v>Configuración de repositorio Git/GitHub, flujo de despliegue a Vercel y ajustes de configuración (vercel.json, conexión con Supabase).</v>
+        <v>Implementación de la bitácora en Excel (Log, Resumen, Versiones, Ref Git y Vercel, Presupuesto) y documentación funcional básica para el uso de la app.</v>
       </c>
       <c r="C8">
-        <v>90000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
+        <v>Integración y despliegue</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Configuración de repositorio Git/GitHub, flujo de despliegue a Vercel y ajustes de configuración (vercel.json, conexión con Supabase).</v>
+      </c>
+      <c r="C9">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>Mantenimiento y soporte inicial</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B10" t="str">
         <v>Soporte post–implementación, pequeños ajustes funcionales y acompañamiento durante el primer período de uso.</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>80000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.15: Filtro Tipo en Todas las transacciones
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1178,9 +1178,26 @@
         <v>Implementacion</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="B46" t="str">
+        <v>12:15</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Filtro Tipo en Todas las transacciones</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Agregar filtro por campo Tipo (Ingreso/Egreso) en la solapa Todas las transacciones. Combina con filtros Mes y Categoría.</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Implementacion</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E45"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E46"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1631,7 +1648,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1817,9 +1834,20 @@
         <v>Solapa Todas las transacciones (filtros mes y categoría); modal edición completa con todos los campos y combos para normalizados</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>1.15</v>
+      </c>
+      <c r="B17" t="str">
+        <v>28/02/2025</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Filtro Tipo (Ingreso/Egreso) en solapa Todas las transacciones</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C17"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v1.16: proyección 3 meses (config, Int. caución en cadena, disclaimer)
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/Bitacora_tareas.xlsx
+++ b/Bitacora_tareas.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1195,16 +1195,50 @@
         <v>Implementacion</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>27/02/2026</v>
+      </c>
+      <c r="B47" t="str">
+        <v>14:00</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Proyección 3 meses e Int. por caución proyectado</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Configuración (Configuración en menú): método Mediana/Promedio y meses de historia (3, 6, 12, 24). Próximos 3 meses proyectados con ventana rodante. Int. por caución: punto de partida = último mes real (G/P + interés), luego última tasa conocida aplicada en cadena para cada mes proyectado.</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Implementacion</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>27/02/2026</v>
+      </c>
+      <c r="B48" t="str">
+        <v>14:15</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Disclaimer bajo proyección</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Texto en letra chica y gris oscuro bajo la proyección indicando metodología: Mediana/Promedio de N meses, ventana rodante, y cómo se calcula Int. por caución proyectado.</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Implementacion</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E48"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1549,9 +1583,33 @@
         <v>Modal de edición con todos los campos: fecha, mes, año, tipo movimiento, monto, moneda, status, medio pago, categoría, cuenta contable, origen archivo, descripción, cliente, cat_desc, id_origen, id_operación. Combos para campos normalizados (valores existentes en BD). editado y editado_detalle al guardar.</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Proyección próximos 3 meses</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Debajo del total real en Flujo por mes: "Próximos 3 meses proyectados" con ventana rodante. Configuración (sidebar): método (Mediana/Promedio) y meses de historia (3, 6, 12, 24). Ingresos, egresos, G/P y ratios proyectados por mes.</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Int. por caución proyectado</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Para cada mes proyectado: punto de partida = G/P + interés del período anterior (último real para mes 1; proyectado 1 para mes 2; proyectado 2 para mes 3). Se aplica la última tasa conocida en cadena. Sin salto respecto al último valor real.</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Disclaimer proyección</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Debajo de las filas proyectadas, texto en letra chica y gris oscuro que explica la metodología: Mediana/Promedio de N meses, ventana rodante, y cálculo de Int. por caución proyectado.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B45"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1648,7 +1706,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1845,9 +1903,20 @@
         <v>Filtro Tipo (Ingreso/Egreso) en solapa Todas las transacciones</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>1.16</v>
+      </c>
+      <c r="B18" t="str">
+        <v>27/02/2026</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Proyección 3 meses: config (mediana/promedio, meses historia), ventana rodante; Int. por caución proyectado con punto de partida = último real (G/P+interés) y última tasa en cadena; disclaimer bajo proyección. Despliegue a producción.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C18"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>